<commit_message>
Update app to include multi-year boxplots, clean foggy days out of data
</commit_message>
<xml_diff>
--- a/data/tower_count/tower_count_2001.xlsx
+++ b/data/tower_count/tower_count_2001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejgna\Documents\project-eleanor-and-wriley\data\tower_count\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7669E1FC-CC61-4EBF-8F88-DA2C6B6F06D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609BA9E4-5E48-4FE3-B49A-A6343552636B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>2 DCCO</t>
-  </si>
-  <si>
-    <t>no count</t>
   </si>
   <si>
     <t>gulls</t>
@@ -485,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +500,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -512,13 +509,13 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -541,35 +538,50 @@
         <v>268</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>37057</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
+        <v>37058</v>
+      </c>
+      <c r="B5">
+        <v>137</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>172</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>37058</v>
+        <v>37061</v>
       </c>
       <c r="B6">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6">
-        <v>6</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
+        <v>35</v>
+      </c>
+      <c r="E6" s="2">
+        <v>97</v>
       </c>
       <c r="F6">
-        <v>172</v>
+        <v>273</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
@@ -577,65 +589,65 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>37061</v>
+        <v>37063</v>
       </c>
       <c r="B7">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D7">
-        <v>35</v>
-      </c>
-      <c r="E7" s="2">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="F7">
-        <v>273</v>
+        <v>183</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>37063</v>
+        <v>37064</v>
       </c>
       <c r="B8">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>142</v>
+      </c>
+      <c r="G8" t="s">
         <v>14</v>
-      </c>
-      <c r="D8">
-        <v>6</v>
-      </c>
-      <c r="F8">
-        <v>183</v>
-      </c>
-      <c r="G8" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>37064</v>
+        <v>37068</v>
       </c>
       <c r="B9">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="F9">
-        <v>142</v>
+        <v>198</v>
       </c>
       <c r="G9" t="s">
         <v>15</v>
@@ -643,238 +655,238 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>37068</v>
+        <v>37069</v>
       </c>
       <c r="B10">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="E10">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F10">
-        <v>198</v>
-      </c>
-      <c r="G10" t="s">
-        <v>16</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>37069</v>
+        <v>37070</v>
       </c>
       <c r="B11">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="E11">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="F11">
-        <v>105</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="P11" s="1"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>37070</v>
+        <v>37071</v>
       </c>
       <c r="B12">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E12">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="F12">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="G12" t="s">
         <v>17</v>
       </c>
-      <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>37071</v>
+        <v>37073</v>
       </c>
       <c r="B13">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13">
-        <v>96</v>
-      </c>
-      <c r="E13">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13">
-        <v>236</v>
-      </c>
-      <c r="G13" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>37073</v>
+        <v>37075</v>
       </c>
       <c r="B14">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14">
-        <v>49</v>
+        <v>72</v>
+      </c>
+      <c r="E14">
+        <v>36</v>
       </c>
       <c r="F14">
-        <v>80</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>37075</v>
+        <v>37076</v>
       </c>
       <c r="B15">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="E15">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F15">
-        <v>226</v>
+        <v>155</v>
+      </c>
+      <c r="G15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>37076</v>
+        <v>37079</v>
       </c>
       <c r="B16">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E16">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F16">
-        <v>155</v>
+        <v>220</v>
       </c>
       <c r="G16" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>37079</v>
+        <v>37086</v>
       </c>
       <c r="B17">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E17">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F17">
-        <v>220</v>
+        <v>175</v>
       </c>
       <c r="G17" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>37086</v>
+        <v>37087</v>
       </c>
       <c r="B18">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="E18">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F18">
-        <v>175</v>
-      </c>
-      <c r="G18" t="s">
-        <v>20</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>37087</v>
+        <v>37090</v>
       </c>
       <c r="B19">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E19">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F19">
-        <v>220</v>
+        <v>270</v>
+      </c>
+      <c r="G19" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>37090</v>
+        <v>37091</v>
       </c>
       <c r="B20">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="E20">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F20">
-        <v>270</v>
+        <v>227</v>
       </c>
       <c r="G20" t="s">
         <v>21</v>
@@ -882,22 +894,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>37091</v>
+        <v>37093</v>
       </c>
       <c r="B21">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E21">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F21">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G21" t="s">
         <v>22</v>
@@ -905,10 +917,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>37093</v>
+        <v>37094</v>
       </c>
       <c r="B22">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -917,34 +929,14 @@
         <v>52</v>
       </c>
       <c r="E22">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F22">
-        <v>225</v>
-      </c>
-      <c r="G22" t="s">
-        <v>23</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>37094</v>
-      </c>
-      <c r="B23">
-        <v>105</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23">
-        <v>52</v>
-      </c>
-      <c r="E23">
-        <v>13</v>
-      </c>
-      <c r="F23">
-        <v>323</v>
-      </c>
+      <c r="A23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
@@ -982,17 +974,14 @@
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>